<commit_message>
ac-bet updated in template
</commit_message>
<xml_diff>
--- a/Projects/INBEVTRADMX/Data/inbevtradmx_template_11_v2.xlsx
+++ b/Projects/INBEVTRADMX/Data/inbevtradmx_template_11_v2.xlsx
@@ -20,6 +20,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">template!$A$1:$W$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">template!$A$1:$W$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">template!$A$1:$W$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">template!$A$1:$W$71</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -396,7 +397,7 @@
     <t xml:space="preserve">product_type, manufacturer_name, store_type, Store Additional Attribute 4, Store Additional Attribute 13, template_name,AC/BET</t>
   </si>
   <si>
-    <t xml:space="preserve">yes</t>
+    <t xml:space="preserve">Yes</t>
   </si>
   <si>
     <t xml:space="preserve">Set FRIA Botella Cerrada Sin Cooler</t>
@@ -1115,40 +1116,40 @@
   </sheetPr>
   <dimension ref="1:71"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V1"/>
-      <selection pane="bottomLeft" activeCell="W3" activeCellId="0" sqref="W3"/>
+      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
+      <selection pane="bottomLeft" activeCell="Z43" activeCellId="0" sqref="Z43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="39.8214285714286"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="78.6989795918367"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="39.1479591836735"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="56.8316326530612"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="147.413265306122"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="161.316326530612"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="3" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="3" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="3" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.0612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="45.4897959183674"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="39.4183673469388"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="77.7551020408163"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="38.6071428571429"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="56.1581632653061"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="145.790816326531"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="159.561224489796"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="3" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="3" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="3" width="7.1530612244898"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -66977,9 +66978,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="7" t="s">
@@ -67104,9 +67102,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">

</xml_diff>

<commit_message>
template att 4 updated
</commit_message>
<xml_diff>
--- a/Projects/INBEVTRADMX/Data/inbevtradmx_template_11_v2.xlsx
+++ b/Projects/INBEVTRADMX/Data/inbevtradmx_template_11_v2.xlsx
@@ -21,6 +21,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">template!$A$1:$W$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">template!$A$1:$W$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">template!$A$1:$W$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">template!$A$1:$W$71</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -250,7 +251,7 @@
     <t xml:space="preserve">ABI-GM, NESTLE, GARCI CRESPO, KERMATO, RED BULL</t>
   </si>
   <si>
-    <t xml:space="preserve">BC, CONCESIONARIOS</t>
+    <t xml:space="preserve">BC, CONCESIONARIO</t>
   </si>
   <si>
     <t xml:space="preserve">CC</t>
@@ -1116,40 +1117,40 @@
   </sheetPr>
   <dimension ref="1:71"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
-      <selection pane="bottomLeft" activeCell="Z43" activeCellId="0" sqref="Z43"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="R12" activeCellId="0" sqref="R9:R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="45.4897959183674"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="39.4183673469388"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="77.7551020408163"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="56.1581632653061"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="145.790816326531"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="159.561224489796"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="31.4540816326531"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="3" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="3" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="3" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="38.8775510204082"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="76.8112244897959"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="55.4795918367347"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="144.173469387755"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="157.80612244898"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="3" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="3" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="3" width="7.02040816326531"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -66974,10 +66975,13 @@
   <dimension ref="B2:E14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="R9:R28 C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="7" t="s">
@@ -67098,10 +67102,13 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="R9:R28 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">

</xml_diff>